<commit_message>
Fixing Ichnocarpus entry on .tre files, spreadsheet, and updating script accordingly.
</commit_message>
<xml_diff>
--- a/Inputs/Supplemental Inputs - Sofia/Spreadsheets/Manual LCVP name standardization.xlsx
+++ b/Inputs/Supplemental Inputs - Sofia/Spreadsheets/Manual LCVP name standardization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaquijada/Documents/McGill/2024 Soper Lab/AusStoich/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaquijada/Documents/McGill/2024 Soper Lab/AusStoich-Collab/Inputs/Supplemental Inputs - Sofia/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D6BBC-F931-1941-A58D-75C9A3AE6FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC99ED2-55F4-9140-9220-5B1E92AD114D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="760" windowWidth="26140" windowHeight="17440" activeTab="2" xr2:uid="{8EB074A1-37CE-C24C-8F19-4DA7AA825B5C}"/>
+    <workbookView xWindow="1240" yWindow="760" windowWidth="26140" windowHeight="17440" firstSheet="1" activeTab="6" xr2:uid="{8EB074A1-37CE-C24C-8F19-4DA7AA825B5C}"/>
   </bookViews>
   <sheets>
     <sheet name="genus resolution" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9465" uniqueCount="2516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9469" uniqueCount="2519">
   <si>
     <t>Acanthaceae Dipteracanthus</t>
   </si>
@@ -7706,6 +7706,15 @@
   </si>
   <si>
     <t>need to get one rep per species in austraits_wo_lcvp_search</t>
+  </si>
+  <si>
+    <t>Ichnocarpus_frutescens</t>
+  </si>
+  <si>
+    <t>Ichnocarpus</t>
+  </si>
+  <si>
+    <t>manually added and fixed on csv as well</t>
   </si>
 </sst>
 </file>
@@ -10482,7 +10491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC8B7BB-70CF-5845-A93D-7BF57A0D3637}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -25969,8 +25978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D648026B-C607-B04B-BA96-0AC790572AA9}">
   <dimension ref="A1:F860"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="F711" sqref="F711"/>
+    <sheetView tabSelected="1" topLeftCell="A813" workbookViewId="0">
+      <selection activeCell="E834" sqref="E834"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -34969,7 +34978,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="817" spans="1:3" ht="16">
+    <row r="817" spans="1:4" ht="16">
       <c r="A817" s="44" t="s">
         <v>1781</v>
       </c>
@@ -34980,7 +34989,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="818" spans="1:3" ht="16">
+    <row r="818" spans="1:4" ht="16">
       <c r="A818" s="44" t="s">
         <v>2450</v>
       </c>
@@ -34991,7 +35000,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="819" spans="1:3" ht="16">
+    <row r="819" spans="1:4" ht="16">
       <c r="A819" s="44" t="s">
         <v>1708</v>
       </c>
@@ -35002,7 +35011,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="820" spans="1:3" ht="16">
+    <row r="820" spans="1:4" ht="16">
       <c r="A820" s="44" t="s">
         <v>1793</v>
       </c>
@@ -35013,7 +35022,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="821" spans="1:3" ht="16">
+    <row r="821" spans="1:4" ht="16">
       <c r="A821" s="44" t="s">
         <v>1705</v>
       </c>
@@ -35024,7 +35033,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="822" spans="1:3" ht="16">
+    <row r="822" spans="1:4" ht="16">
       <c r="A822" s="44" t="s">
         <v>1803</v>
       </c>
@@ -35035,7 +35044,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="823" spans="1:3" ht="16">
+    <row r="823" spans="1:4" ht="16">
       <c r="A823" s="44" t="s">
         <v>2286</v>
       </c>
@@ -35046,7 +35055,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="824" spans="1:3" ht="16">
+    <row r="824" spans="1:4" ht="16">
       <c r="A824" s="44" t="s">
         <v>1868</v>
       </c>
@@ -35057,7 +35066,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="825" spans="1:3" ht="16">
+    <row r="825" spans="1:4" ht="16">
       <c r="A825" s="44" t="s">
         <v>228</v>
       </c>
@@ -35068,7 +35077,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="826" spans="1:3" ht="16">
+    <row r="826" spans="1:4" ht="16">
       <c r="A826" s="44" t="s">
         <v>229</v>
       </c>
@@ -35079,7 +35088,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="827" spans="1:3" ht="16">
+    <row r="827" spans="1:4" ht="16">
       <c r="A827" s="44" t="s">
         <v>2290</v>
       </c>
@@ -35090,7 +35099,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="828" spans="1:3" ht="16">
+    <row r="828" spans="1:4" ht="16">
       <c r="A828" s="44" t="s">
         <v>1961</v>
       </c>
@@ -35101,7 +35110,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="829" spans="1:3" ht="16">
+    <row r="829" spans="1:4" ht="16">
       <c r="A829" s="44" t="s">
         <v>2287</v>
       </c>
@@ -35112,7 +35121,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="830" spans="1:3" ht="16">
+    <row r="830" spans="1:4" ht="16">
       <c r="A830" s="44" t="s">
         <v>2288</v>
       </c>
@@ -35123,7 +35132,21 @@
         <v>204</v>
       </c>
     </row>
-    <row r="832" spans="1:3" ht="16">
+    <row r="831" spans="1:4">
+      <c r="A831" s="43" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B831" s="43" t="s">
+        <v>2517</v>
+      </c>
+      <c r="C831" s="43" t="s">
+        <v>430</v>
+      </c>
+      <c r="D831" s="43" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="832" spans="1:4" ht="16">
       <c r="A832"/>
       <c r="B832"/>
       <c r="C832"/>

</xml_diff>